<commit_message>
RunnerSingleScenario visa rel delta so
</commit_message>
<xml_diff>
--- a/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=7, region=se3].xlsx
+++ b/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=7, region=se3].xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>0</t>
   </si>
@@ -29,6 +29,9 @@
     <t>4</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>Scenario</t>
   </si>
   <si>
@@ -44,25 +47,34 @@
     <t>Adj. rev.</t>
   </si>
   <si>
+    <t>dSoH (ppm)</t>
+  </si>
+  <si>
     <t>G2V</t>
   </si>
   <si>
-    <t>-6.6</t>
+    <t>-4.1</t>
   </si>
   <si>
     <t>-0</t>
   </si>
   <si>
+    <t>56.1</t>
+  </si>
+  <si>
     <t>V2G</t>
   </si>
   <si>
-    <t>3.7</t>
-  </si>
-  <si>
-    <t>-0.1</t>
-  </si>
-  <si>
-    <t>3.6</t>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>-0.6</t>
+  </si>
+  <si>
+    <t>-3.6</t>
+  </si>
+  <si>
+    <t>50.3</t>
   </si>
 </sst>
 </file>
@@ -107,7 +119,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -118,6 +130,7 @@
     <col min="3" max="3" width="11.69140625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="8.55078125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="12.9609375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="8.45703125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -136,25 +149,31 @@
       <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
+      <c r="F1" t="s" s="0">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -162,19 +181,22 @@
         <v>1.0</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>0</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -182,19 +204,22 @@
         <v>2.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>0</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dSoH V2G mindre än för G2V
</commit_message>
<xml_diff>
--- a/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=7, region=se3].xlsx
+++ b/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=7, region=se3].xlsx
@@ -53,28 +53,28 @@
     <t>G2V</t>
   </si>
   <si>
-    <t>-4.1</t>
+    <t>-6.5</t>
   </si>
   <si>
     <t>-0</t>
   </si>
   <si>
-    <t>56.1</t>
+    <t>50</t>
   </si>
   <si>
     <t>V2G</t>
   </si>
   <si>
-    <t>-3</t>
+    <t>-0.9</t>
   </si>
   <si>
     <t>-0.6</t>
   </si>
   <si>
-    <t>-3.6</t>
-  </si>
-  <si>
-    <t>50.3</t>
+    <t>-1.5</t>
+  </si>
+  <si>
+    <t>54.5</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
CorrectedActionPenalizer som del av mediator
</commit_message>
<xml_diff>
--- a/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=7, region=se3].xlsx
+++ b/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=7, region=se3].xlsx
@@ -65,16 +65,16 @@
     <t>V2G</t>
   </si>
   <si>
-    <t>-0.9</t>
+    <t>-1</t>
   </si>
   <si>
     <t>-0.6</t>
   </si>
   <si>
-    <t>-1.5</t>
-  </si>
-  <si>
-    <t>61.3</t>
+    <t>-1.6</t>
+  </si>
+  <si>
+    <t>61.2</t>
   </si>
 </sst>
 </file>

</xml_diff>